<commit_message>
- Updated Excel backup and template - Updated Excel File Structure file to include Output columns
</commit_message>
<xml_diff>
--- a/src/test/java/Excel/FlightData_Backup.xlsx
+++ b/src/test/java/Excel/FlightData_Backup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel Nezic\IdeaProjects\CucumberIAG\src\test\java\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4DD25D-FBB6-4588-8ACC-53DAB668EA03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A3D7C3F-71F2-460B-AD6A-9958BA3814D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{15C5D190-8B55-41A7-AE81-1E037CBB6904}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
   <si>
     <t>Flight Type</t>
   </si>
@@ -125,6 +125,93 @@
   </si>
   <si>
     <t>Message</t>
+  </si>
+  <si>
+    <t>Entry</t>
+  </si>
+  <si>
+    <t>Timestamp</t>
+  </si>
+  <si>
+    <t>Base Fare</t>
+  </si>
+  <si>
+    <t>Fee/Surcharge</t>
+  </si>
+  <si>
+    <t>Addons</t>
+  </si>
+  <si>
+    <t>Total Amount</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>₹1,21,420</t>
+  </si>
+  <si>
+    <t>₹8,332</t>
+  </si>
+  <si>
+    <t>₹10</t>
+  </si>
+  <si>
+    <t>₹1,29,762</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Arrival location 1 does not match dataset</t>
+  </si>
+  <si>
+    <t>Fare elements not found</t>
+  </si>
+  <si>
+    <t>No flight results</t>
+  </si>
+  <si>
+    <t>19/01/2022 11:43:05 am</t>
+  </si>
+  <si>
+    <t>19/01/2022 11:43:12 am</t>
+  </si>
+  <si>
+    <t>19/01/2022 11:43:39 am</t>
+  </si>
+  <si>
+    <t>1,018,020</t>
+  </si>
+  <si>
+    <t>38,556</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>868,618</t>
+  </si>
+  <si>
+    <t>19/01/2022 11:44:07 am</t>
+  </si>
+  <si>
+    <t>19/01/2022 11:45:11 am</t>
+  </si>
+  <si>
+    <t>19/01/2022 11:45:32 am</t>
+  </si>
+  <si>
+    <t>97,330</t>
+  </si>
+  <si>
+    <t>8,938</t>
+  </si>
+  <si>
+    <t>106,274</t>
   </si>
 </sst>
 </file>
@@ -175,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -183,6 +270,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -498,249 +598,265 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354668D4-D94F-4400-B0BC-72EF38E5F017}">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="7.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.140625" style="2"/>
-    <col min="9" max="9" width="7.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="19" style="2" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="20.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="25.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="20.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="25.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="17" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="2" width="11.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="7.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="20.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="25.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="20.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="25.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="3">
+      <c r="F2" s="3">
         <v>25012022</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3">
         <v>3</v>
-      </c>
-      <c r="H2" s="3">
-        <v>1</v>
       </c>
       <c r="I2" s="3">
         <v>1</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="3">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="Q2" s="3"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F3" s="3">
         <v>25022022</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="3">
         <v>27022022</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3" s="3">
         <v>1</v>
-      </c>
-      <c r="H3" s="3">
-        <v>0</v>
       </c>
       <c r="I3" s="3">
         <v>0</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="Q3" s="3"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="3">
+      <c r="C4" s="3">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="3">
+      <c r="F4" s="3">
         <v>25012022</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="6"/>
+      <c r="H4" s="3">
         <v>2</v>
       </c>
-      <c r="H4" s="3">
+      <c r="I4" s="3">
         <v>4</v>
       </c>
-      <c r="I4" s="3">
+      <c r="J4" s="3">
         <v>0</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="3">
+      <c r="M4" s="3">
         <v>27012022</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="3">
+      <c r="O4" s="3">
         <v>28012022</v>
       </c>
-      <c r="O4" s="3"/>
       <c r="P4" s="3"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="Q4" s="3"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="3">
+      <c r="F5" s="3">
         <v>25012022</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3">
+      <c r="G5" s="3"/>
+      <c r="H5" s="3">
         <v>1</v>
       </c>
-      <c r="H5" s="3">
+      <c r="I5" s="3">
         <v>0</v>
       </c>
-      <c r="I5" s="3">
+      <c r="J5" s="3">
         <v>1</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="K5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="Q5" s="3"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="3">
+      <c r="F6" s="3">
         <v>25022022</v>
       </c>
-      <c r="F6" s="3">
+      <c r="G6" s="3">
         <v>27022022</v>
-      </c>
-      <c r="G6" s="3">
-        <v>2</v>
       </c>
       <c r="H6" s="3">
         <v>2</v>
@@ -748,57 +864,63 @@
       <c r="I6" s="3">
         <v>2</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="3">
+        <v>2</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="Q6" s="3"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="3">
+      <c r="C7" s="3">
         <v>1</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="3">
+      <c r="F7" s="3">
         <v>25012022</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3">
-        <v>1</v>
-      </c>
+      <c r="G7" s="3"/>
       <c r="H7" s="3">
         <v>1</v>
       </c>
       <c r="I7" s="3">
         <v>1</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="3">
+        <v>1</v>
+      </c>
+      <c r="K7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="L7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="3">
+      <c r="M7" s="3">
         <v>27012022</v>
       </c>
-      <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q7" s="3"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -815,6 +937,25 @@
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
+      <c r="Q8" s="6"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -824,24 +965,168 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{116CE802-AF6A-49F4-92A0-B86909AD8334}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="40.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="21.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="37.85546875" style="5" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="D1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>